<commit_message>
add excel test files
</commit_message>
<xml_diff>
--- a/bin/role1.xlsx
+++ b/bin/role1.xlsx
@@ -4,19 +4,389 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="4560" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="role" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>作者</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G32" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>光明</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G35" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">黑暗
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="28">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -236,6 +606,68 @@
   </si>
   <si>
     <t>[["aaaa","2.0"],[bbbbb,3.1],[ccc,4d,4f,43,4d,4d,4d,4d]]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>camp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>职业</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camp_Light</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Camp_Dark</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CampType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>job</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>role.jobtype</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>common_0</t>
+  </si>
+  <si>
+    <t>swordman_2</t>
+  </si>
+  <si>
+    <t>array&lt;role.jobtype&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>job2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group&lt;role.jobtype&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group&lt;CampType&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>array&lt;CampType&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>camp_array</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>camp_group</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +675,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +717,21 @@
       <name val="等线"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -306,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -321,6 +768,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -624,11 +1072,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="3" max="3" width="78.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -640,7 +1091,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
@@ -652,7 +1105,9 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
@@ -664,7 +1119,9 @@
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -676,7 +1133,9 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
@@ -686,7 +1145,9 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
@@ -696,7 +1157,9 @@
         <v>8</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
@@ -704,7 +1167,9 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
@@ -714,7 +1179,9 @@
         <v>9</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
@@ -726,7 +1193,9 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
@@ -736,7 +1205,9 @@
         <v>10</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
@@ -748,7 +1219,9 @@
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
@@ -760,7 +1233,9 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1"/>
@@ -793,15 +1268,382 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="3" max="3" width="24.25" customWidth="1"/>
+    <col min="4" max="6" width="25.25" customWidth="1"/>
+    <col min="7" max="8" width="35.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="B29" s="1">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
+        <v>6</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
+        <v>7</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1">
+        <v>8</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1">
+        <v>9</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="5:7">
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="5:7">
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -815,5 +1657,6 @@
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add cpp manager class maker Signed-off-by: love19862003 <love19862003@163.com>
</commit_message>
<xml_diff>
--- a/bin/role1.xlsx
+++ b/bin/role1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -669,6 +669,18 @@
   <si>
     <t>camp_group</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1070,18 +1082,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="3" width="78.125" customWidth="1"/>
+    <col min="4" max="4" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1094,8 +1107,14 @@
       <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1108,8 +1127,14 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1123,7 +1148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1136,8 +1161,14 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1148,8 +1179,14 @@
       <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1160,8 +1197,14 @@
       <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1170,8 +1213,14 @@
       <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1182,8 +1231,14 @@
       <c r="D8" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1196,8 +1251,14 @@
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1208,8 +1269,14 @@
       <c r="D10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1222,8 +1289,14 @@
       <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1236,26 +1309,32 @@
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:6">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:6">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1271,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
aaaaaaaaaaaaaaaaa Signed-off-by: love19862003 <love19862003@163.com>
</commit_message>
<xml_diff>
--- a/bin/role1.xlsx
+++ b/bin/role1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
@@ -66,327 +66,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="E29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G29" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G31" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G32" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E33" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F33" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G33" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>光明</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E34" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F34" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G34" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E35" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F35" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G35" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">黑暗
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -614,10 +299,6 @@
   </si>
   <si>
     <t>职业</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Camp_Light</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -687,7 +368,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,14 +408,6 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="等线"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1084,7 +757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1105,13 +778,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1125,13 +798,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1145,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1159,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1177,7 +850,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1195,7 +868,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1211,7 +884,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1229,7 +902,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1249,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -1267,7 +940,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -1287,7 +960,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>8</v>
@@ -1307,7 +980,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>9</v>
@@ -1350,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1377,16 +1050,16 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1400,19 +1073,19 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1435,10 +1108,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1450,19 +1123,19 @@
         <v>7</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1476,180 +1149,78 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="B29" s="1">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9">
-      <c r="B30" s="1">
-        <v>4</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9">
-      <c r="B31" s="1">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1"/>
-      <c r="B32" s="1">
-        <v>6</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1"/>
-      <c r="B33" s="1">
-        <v>7</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="5"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1"/>
-      <c r="B34" s="1">
-        <v>8</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1"/>
-      <c r="B35" s="1">
-        <v>9</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1"/>

</xml_diff>

<commit_message>
add test self define coordinate type.lua
Signed-off-by: love19862003 <love19862003@163.com>
</commit_message>
<xml_diff>
--- a/bin/role1.xlsx
+++ b/bin/role1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="8775" yWindow="2745" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="monster" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -361,6 +361,68 @@
   </si>
   <si>
     <t>sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coordinate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array&lt;coordinate&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group&lt;coordinate&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,2,3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1,2,3],[1,2,3,4],[1,2,3]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[2]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[3]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[4]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[5]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[6]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[7]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3],[1,2]},{[1],[8]}</t>
+  </si>
+  <si>
+    <t>{[1,2,3,4],[1,2]},{[1],[9]}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -755,19 +817,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="78.125" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
     <col min="4" max="4" width="23.25" customWidth="1"/>
+    <col min="7" max="7" width="14.75" customWidth="1"/>
+    <col min="8" max="8" width="38.5" customWidth="1"/>
+    <col min="9" max="9" width="126.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,8 +851,17 @@
       <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -806,8 +880,17 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -821,7 +904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -840,8 +923,11 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -858,8 +944,17 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -876,8 +971,11 @@
       <c r="F6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -892,8 +990,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -910,8 +1011,11 @@
       <c r="F8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -930,8 +1034,11 @@
       <c r="F9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -948,8 +1055,11 @@
       <c r="F10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -968,8 +1078,11 @@
       <c r="F11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -988,26 +1101,29 @@
       <c r="F12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:9">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:9">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:9">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1023,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add test boolean type
Signed-off-by: love19862003 <love19862003@163.com>
</commit_message>
<xml_diff>
--- a/bin/role1.xlsx
+++ b/bin/role1.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="73">
   <si>
     <t>id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -423,6 +423,101 @@
   </si>
   <si>
     <t>{[1,2,3,4],[1,2]},{[1],[9]}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>array&lt;int&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11,11,11,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group&lt;int&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,14]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,15]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,16]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,17]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,18]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,19]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,20]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,21]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,22]</t>
+  </si>
+  <si>
+    <t>[11,12,13],[11,12,23]</t>
+  </si>
+  <si>
+    <t>array&lt;bool&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[true,false,true]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[true,true]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[true]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group&lt;bool&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[true,false],[true,false],[true,false],[true,false]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -817,22 +912,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
     <col min="4" max="4" width="23.25" customWidth="1"/>
     <col min="7" max="7" width="14.75" customWidth="1"/>
     <col min="8" max="8" width="38.5" customWidth="1"/>
-    <col min="9" max="9" width="126.375" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.625" customWidth="1"/>
+    <col min="12" max="12" width="16.75" customWidth="1"/>
+    <col min="14" max="14" width="53.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,8 +960,23 @@
       <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -889,8 +1004,23 @@
       <c r="I2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -904,7 +1034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -926,8 +1056,23 @@
       <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -953,8 +1098,23 @@
       <c r="I5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -974,8 +1134,23 @@
       <c r="I6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -993,8 +1168,23 @@
       <c r="I7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1014,8 +1204,23 @@
       <c r="I8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8">
+        <v>4</v>
+      </c>
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1037,8 +1242,23 @@
       <c r="I9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1058,8 +1278,23 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1081,8 +1316,23 @@
       <c r="I11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" t="s">
+        <v>64</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1104,8 +1354,23 @@
       <c r="I12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" t="s">
+        <v>64</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1113,20 +1378,35 @@
       <c r="I13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L13" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:14">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:14">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>